<commit_message>
Will be back again
</commit_message>
<xml_diff>
--- a/Remind_data.xlsx
+++ b/Remind_data.xlsx
@@ -367,7 +367,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,7 +393,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>6.25E-2</v>
+        <v>0.20902777777777778</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Solved the issue of comparing the time
</commit_message>
<xml_diff>
--- a/Remind_data.xlsx
+++ b/Remind_data.xlsx
@@ -367,7 +367,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,7 +393,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>0.20902777777777778</v>
+        <v>0.85763888888888884</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Program is now notifing
</commit_message>
<xml_diff>
--- a/Remind_data.xlsx
+++ b/Remind_data.xlsx
@@ -367,7 +367,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -393,7 +393,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>0.85763888888888884</v>
+        <v>0.87638888888888899</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
lets start to work
</commit_message>
<xml_diff>
--- a/Remind_data.xlsx
+++ b/Remind_data.xlsx
@@ -16,15 +16,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>Abhinav</t>
+    <t>Test 1</t>
   </si>
   <si>
-    <t>sibam</t>
+    <t>Test 2</t>
   </si>
   <si>
-    <t>Startup the pc right now sir</t>
+    <t>Test 3</t>
+  </si>
+  <si>
+    <t>Test 4</t>
   </si>
 </sst>
 </file>
@@ -364,7 +367,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -377,7 +380,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>0.66597222222222219</v>
+        <v>0.44097222222222227</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -385,7 +388,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0.10416666666666667</v>
+        <v>0.44166666666666665</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -393,10 +396,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>0.87638888888888899</v>
+        <v>0.44236111111111115</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>0.44305555555555554</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
time.sleep is not working wanna fixed it
</commit_message>
<xml_diff>
--- a/Remind_data.xlsx
+++ b/Remind_data.xlsx
@@ -370,7 +370,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -380,7 +380,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>0.44097222222222227</v>
+        <v>0.46736111111111112</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -388,7 +388,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0.44166666666666665</v>
+        <v>0.4694444444444445</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -396,7 +396,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>0.44236111111111115</v>
+        <v>0.46666666666666662</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -404,7 +404,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>0.44305555555555554</v>
+        <v>0.46875</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Test 1 completed passed
</commit_message>
<xml_diff>
--- a/Remind_data.xlsx
+++ b/Remind_data.xlsx
@@ -21,13 +21,13 @@
     <t>Test 3</t>
   </si>
   <si>
-    <t>Bhia chal thoda pani se akh tho le</t>
+    <t>Test 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Test kr le bhai kam </t>
+    <t>Test 2</t>
   </si>
   <si>
-    <t>20-20-20 eyes Excersise</t>
+    <t>Test 4</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>0.65625</v>
+        <v>0.84166666666666667</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -388,7 +388,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0.64930555555555558</v>
+        <v>0.84236111111111101</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -396,7 +396,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>0.65138888888888891</v>
+        <v>0.84375</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -404,7 +404,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>0.65277777777777779</v>
+        <v>0.84027777777777779</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>

</xml_diff>